<commit_message>
tested symlex android and windows for new release
</commit_message>
<xml_diff>
--- a/apps/features/backlog/android/server_list/server_list.xlsx
+++ b/apps/features/backlog/android/server_list/server_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\office\SymlexVPNTestCases\apps\features\backlog\android\server_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752B713A-DF5D-41AE-A9CD-54B3691D8915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26AF41F2-CF5C-4310-ACA5-0B6BA8A7F613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -213,9 +213,6 @@
   </si>
   <si>
     <t>the server page displays the list of available vpn servers.</t>
-  </si>
-  <si>
-    <t>verify that the search functionality works as expected, accurately displaying the matching server.</t>
   </si>
   <si>
     <t>verify that the vpn app successfully disconnects to a gaming server.</t>
@@ -552,6 +549,9 @@
 4. navigate to the vpn connection page
 5. goto to search place holder
 6. try to check the search placeholder for copy paste option</t>
+  </si>
+  <si>
+    <t>verify that the search functionality works as expected, accurately displaying the searching matching server.</t>
   </si>
 </sst>
 </file>
@@ -1753,8 +1753,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1874,16 +1874,16 @@
         <v>8</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>9</v>
@@ -1916,13 +1916,13 @@
         <v>10</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>62</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>63</v>
@@ -1956,16 +1956,16 @@
         <v>11</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>64</v>
+        <v>126</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>9</v>
@@ -1996,16 +1996,16 @@
         <v>12</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>9</v>
@@ -2036,13 +2036,13 @@
         <v>13</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>14</v>
@@ -2076,13 +2076,13 @@
         <v>15</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>16</v>
@@ -2116,16 +2116,16 @@
         <v>17</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>9</v>
@@ -2156,16 +2156,16 @@
         <v>18</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>9</v>
@@ -2196,16 +2196,16 @@
         <v>19</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>9</v>
@@ -2236,16 +2236,16 @@
         <v>20</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>9</v>
@@ -2276,13 +2276,13 @@
         <v>21</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>22</v>
@@ -2316,16 +2316,16 @@
         <v>23</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>9</v>
@@ -2356,16 +2356,16 @@
         <v>24</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="D16" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>9</v>
@@ -2396,16 +2396,16 @@
         <v>25</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>9</v>
@@ -2436,16 +2436,16 @@
         <v>26</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>9</v>
@@ -2476,13 +2476,13 @@
         <v>27</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>29</v>
@@ -2516,13 +2516,13 @@
         <v>31</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>30</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>32</v>
@@ -2556,13 +2556,13 @@
         <v>33</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>35</v>
@@ -2596,13 +2596,13 @@
         <v>36</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>38</v>
@@ -2636,13 +2636,13 @@
         <v>39</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>42</v>
@@ -2676,13 +2676,13 @@
         <v>44</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>41</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>43</v>
@@ -2716,16 +2716,16 @@
         <v>46</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>45</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>9</v>
@@ -2756,16 +2756,16 @@
         <v>48</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>47</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>9</v>
@@ -2796,13 +2796,13 @@
         <v>51</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>49</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>50</v>
@@ -2836,13 +2836,13 @@
         <v>53</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>52</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>54</v>
@@ -2876,13 +2876,13 @@
         <v>55</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>56</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>57</v>
@@ -2914,13 +2914,13 @@
         <v>59</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>60</v>
@@ -2949,19 +2949,19 @@
     </row>
     <row r="31" spans="1:26" ht="108" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C31" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>126</v>
-      </c>
       <c r="E31" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>9</v>
@@ -2989,19 +2989,19 @@
     </row>
     <row r="32" spans="1:26" ht="119.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F32" s="17" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
connection page ui test case written
</commit_message>
<xml_diff>
--- a/apps/features/backlog/android/server_list/server_list.xlsx
+++ b/apps/features/backlog/android/server_list/server_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\office\SymlexVPNTestCases\apps\features\backlog\android\server_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26AF41F2-CF5C-4310-ACA5-0B6BA8A7F613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBC0B48-592C-45DA-9A0A-41F52BD0A58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="130">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -552,6 +552,21 @@
   </si>
   <si>
     <t>verify that the search functionality works as expected, accurately displaying the searching matching server.</t>
+  </si>
+  <si>
+    <t>TC_SYM_SP_031</t>
+  </si>
+  <si>
+    <t>check free server is working properly or not</t>
+  </si>
+  <si>
+    <t>1. go to playstore and install symlexvpn in the mobile
+2. open the installed symlexvpn application.
+3. login with proper credentials as free user
+4. navigate to the vpn server list page
+5. go for free server
+6. try to connect to the free server
+7. also check if the same server wroking properly for a premium user/ check the free server and same server in premium account working properly or not</t>
   </si>
 </sst>
 </file>
@@ -1535,7 +1550,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G32" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G33" dataDxfId="7">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Case ID" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites" dataDxfId="5"/>
@@ -1753,8 +1768,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3028,13 +3043,25 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="144" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
+      <c r="A33" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="16"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -29859,7 +29886,7 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F5:F32" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F5:F33" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>